<commit_message>
update system test case
</commit_message>
<xml_diff>
--- a/adhafera/test/system_test.xlsx
+++ b/adhafera/test/system_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="正常系" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -61,6 +61,37 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>状態</t>
+    <rPh sb="0" eb="2">
+      <t>ジョウタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>取消ボタンを押下</t>
+    <rPh sb="0" eb="2">
+      <t>トリケシ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>オウカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>シナリオ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>家計簿を登録する</t>
+    <rPh sb="0" eb="3">
+      <t>カケイボ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>トウロク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>登録ボタンを押下</t>
     <rPh sb="0" eb="2">
       <t>トウロク</t>
@@ -71,9 +102,244 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>状態</t>
+    <t>家計簿情報を入力</t>
+    <rPh sb="0" eb="5">
+      <t>カケイボジョウホウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日付: "2015-01-01"
+内容: "テスト用データ"
+カテゴリ: "テスト"
+金額: "100"
+ボタン: "収入"を選択</t>
     <rPh sb="0" eb="2">
-      <t>ジョウタイ</t>
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>家計簿の登録を取り消す</t>
+    <rPh sb="0" eb="3">
+      <t>カケイボ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ケ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>家計簿情報を入力</t>
+    <rPh sb="0" eb="5">
+      <t>カケイボジョウホウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日付: "2015-01-01"
+内容: "テスト用データ"
+ボタン: "収入"を選択</t>
+    <rPh sb="0" eb="2">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>未入力の項目がある</t>
+    <rPh sb="0" eb="3">
+      <t>ミニュウリョク</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>コウモク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリを起動</t>
+    <rPh sb="4" eb="6">
+      <t>キドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>家計簿情報を入力</t>
+    <rPh sb="0" eb="3">
+      <t>カケイボ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日付: "2015-01-01"
+カテゴリ: "テスト"
+金額: "100"
+ボタン: "収入"を選択</t>
+    <rPh sb="0" eb="2">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>不正な値がある</t>
+    <rPh sb="0" eb="2">
+      <t>フセイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・入力欄には何も表示されていない
+・テーブルは"支出"が選択されている
+・全てのチェックマークが表示されていない</t>
+    <rPh sb="1" eb="4">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>シシュツ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・画面に"内容が入力されていません"と書かれたToastが表示されている
+・内容の項目にチェックマークが表示されている
+・テーブルは"収入"が選択されている</t>
+    <rPh sb="1" eb="3">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="67" eb="69">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・画面に"日付が不正です"と書かれたToastが表示されている
+・日付の項目にチェックマークが表示されている
+・テーブルは"収入"が選択されている</t>
+    <rPh sb="1" eb="3">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>フセイ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="47" eb="49">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>センタク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -88,381 +354,173 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>日付: '2015-01-01'
-内容: 'テスト用データ'
-カテゴリ: 'テスト'
-金額: '100'
-ボタン: '収入'を選択</t>
+    <t>・画面に"家計簿が登録されました"と書かれたToastが表示されている
+・入力欄には何も表示されていない
+・テーブルは"収入"が選択されている
+・全てのチェックマークが表示されていない</t>
+    <rPh sb="1" eb="3">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="5" eb="8">
+      <t>カケイボ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="37" eb="40">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="60" eb="62">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="73" eb="74">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="84" eb="86">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・入力欄には何も表示されていない
+・テーブルは"収入"が選択されている
+・全てのチェックマークが表示されていない</t>
+    <rPh sb="1" eb="4">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・入力欄には何も表示されていない
+・テーブルは"収入"が選択されている
+・全てのチェックマークが表示されていない</t>
+    <rPh sb="1" eb="4">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>不正な値をもつ項目が含まれている</t>
+    <rPh sb="0" eb="2">
+      <t>フセイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>フク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日付: "2015-01-01"
+内容: "テスト用データ"
+カテゴリ: "テスト"
+金額: "不正な金額"
+ボタン: "収入"を選択</t>
     <rPh sb="0" eb="2">
       <t>ヒヅケ</t>
     </rPh>
     <rPh sb="17" eb="19">
       <t>ナイヨウ</t>
     </rPh>
-    <rPh sb="25" eb="26">
-      <t>ヨウ</t>
-    </rPh>
     <rPh sb="43" eb="45">
       <t>キンガク</t>
     </rPh>
-    <rPh sb="59" eb="61">
+    <rPh sb="48" eb="50">
+      <t>フセイ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="61" eb="63">
       <t>シュウニュウ</t>
     </rPh>
-    <rPh sb="63" eb="65">
+    <rPh sb="65" eb="67">
       <t>センタク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>日付: '2015-01-01'
-内容: 'テスト用データ'
-ボタン: '収入'を選択</t>
+    <t>日付: "不正な日付"
+内容: "テスト用データ"
+カテゴリ: "テスト"
+金額: "100"
+ボタン: "収入"を選択</t>
     <rPh sb="0" eb="2">
       <t>ヒヅケ</t>
     </rPh>
-    <rPh sb="17" eb="19">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>シュウニュウ</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>センタク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>日付: '2015-01-01'
-内容: 'テスト用データ'
-ボタン: '支出'を選択</t>
-    <rPh sb="0" eb="2">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>シシュツ</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>センタク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・'カテゴリ, 金額を入力してください'と表示されていること
-・カテゴリの入力欄の横にマークが表示されていること
-・金額の入力欄の横にマークが表示されていること</t>
-    <rPh sb="8" eb="10">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="37" eb="40">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="41" eb="42">
-      <t>ヨコ</t>
-    </rPh>
-    <rPh sb="47" eb="49">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="61" eb="64">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="65" eb="66">
-      <t>ヨコ</t>
-    </rPh>
-    <rPh sb="71" eb="73">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・'日付が不正です'と表示されていること
-・日付の入力欄の横にマークが表示されていること</t>
-    <rPh sb="2" eb="4">
-      <t>ヒヅケ</t>
-    </rPh>
     <rPh sb="5" eb="7">
       <t>フセイ</t>
     </rPh>
-    <rPh sb="11" eb="13">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="25" eb="28">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>ヨコ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・'金額が不正です'と表示されていること
-・金額の入力欄の横にマークが表示されていること</t>
-    <rPh sb="2" eb="4">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>フセイ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="25" eb="28">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>ヨコ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>日付: '不正な日付'
-内容: 'テスト用データ'
-カテゴリ: 'テスト'
-金額: '100'
-ボタン: '支出'を選択</t>
-    <rPh sb="0" eb="2">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>フセイ</t>
-    </rPh>
     <rPh sb="8" eb="10">
       <t>ヒヅケ</t>
     </rPh>
     <rPh sb="12" eb="14">
       <t>ナイヨウ</t>
     </rPh>
-    <rPh sb="20" eb="21">
-      <t>ヨウ</t>
-    </rPh>
     <rPh sb="38" eb="40">
       <t>キンガク</t>
     </rPh>
     <rPh sb="54" eb="56">
-      <t>シシュツ</t>
+      <t>シュウニュウ</t>
     </rPh>
     <rPh sb="58" eb="60">
       <t>センタク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>日付: '2015-01-01'
-内容: 'テスト用データ'
-カテゴリ: 'テスト'
-金額: '不正な金額'
-ボタン: '支出'を選択</t>
-    <rPh sb="0" eb="2">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="43" eb="45">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>フセイ</t>
-    </rPh>
-    <rPh sb="51" eb="53">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>シシュツ</t>
-    </rPh>
-    <rPh sb="65" eb="67">
-      <t>センタク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>日付: '01-01-2015'
-内容: 'テスト用データ'
-カテゴリ: 'テスト'
-金額: '-100'
-ボタン: '支出'を選択</t>
-    <rPh sb="0" eb="2">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="43" eb="45">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="60" eb="62">
-      <t>シシュツ</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>センタク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・'日付, 金額が不正です'と表示されていること
-・日付の入力欄の横にマークが表示されていること
-・金額の入力欄の横にマークが表示されていること</t>
-    <rPh sb="2" eb="4">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>フセイ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="29" eb="32">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>ヨコ</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="50" eb="52">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="53" eb="56">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="57" eb="58">
-      <t>ヨコ</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・入力欄には何も表示されていないこと
-・テーブルは'支出'が選択されていること
-・全てのチェックマークが表示されていないこと</t>
-    <rPh sb="1" eb="4">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>ナニ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>シシュツ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="41" eb="42">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="52" eb="54">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・'家計簿が登録されました'と表示されていること
-・入力欄には何も表示されていないこと
-・テーブルは'収入'が選択されていること
-・全てのチェックマークが表示されていないこと</t>
-    <rPh sb="2" eb="5">
-      <t>カケイボ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>トウロク</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="26" eb="29">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="31" eb="32">
-      <t>ナニ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="51" eb="53">
-      <t>シュウニュウ</t>
-    </rPh>
-    <rPh sb="55" eb="57">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="66" eb="67">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="77" eb="79">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・入力欄には何も表示されていないこと
-・テーブルは'収入'が選択されていること
-・全てのチェックマークが表示されていないこと</t>
-    <rPh sb="1" eb="4">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>ナニ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>シュウニュウ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="41" eb="42">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="52" eb="54">
-      <t>ヒョウジ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -520,7 +578,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -587,7 +645,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -597,6 +668,36 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -609,7 +710,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -618,13 +719,113 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -633,15 +834,13 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -651,122 +850,14 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="189">
+  <cellStyleXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -956,58 +1047,100 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="189">
+  <cellStyles count="199">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -1102,6 +1235,11 @@
     <cellStyle name="ハイパーリンク" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -1197,6 +1335,11 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="198" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1525,22 +1668,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G6"/>
+  <dimension ref="B1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.1640625" customWidth="1"/>
-    <col min="4" max="4" width="47.1640625" customWidth="1"/>
-    <col min="5" max="5" width="37.83203125" customWidth="1"/>
-    <col min="6" max="7" width="47.1640625" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="47.1640625" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="37.83203125" customWidth="1"/>
+    <col min="8" max="8" width="56.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="19" thickBot="1"/>
-    <row r="2" spans="2:7" ht="19" thickBot="1">
+    <row r="1" spans="2:8" ht="19" thickBot="1"/>
+    <row r="2" spans="2:8" ht="19" thickBot="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1548,89 +1693,224 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="44">
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="12"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="2:8" ht="70">
+      <c r="B5" s="13"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="44">
+      <c r="B6" s="20">
+        <v>2</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="12"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="2:8" ht="70">
+      <c r="B8" s="13"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="44">
+      <c r="B9" s="20">
+        <v>3</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="12"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="2:8" ht="44">
+      <c r="B11" s="13"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="44">
+      <c r="B12" s="20">
+        <v>4</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" s="12"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="2:8" ht="71" thickBot="1">
+      <c r="B14" s="21"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="44">
-      <c r="B3" s="8">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="70">
-      <c r="B4" s="8">
-        <v>2</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="70">
-      <c r="B5" s="8">
-        <v>3</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="45" thickBot="1">
-      <c r="B6" s="13">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19" t="s">
-        <v>22</v>
+      <c r="G14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B11"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1644,23 +1924,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G6"/>
+  <dimension ref="B1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.1640625" customWidth="1"/>
-    <col min="4" max="4" width="47.1640625" customWidth="1"/>
-    <col min="5" max="5" width="37.83203125" customWidth="1"/>
-    <col min="6" max="6" width="47.1640625" customWidth="1"/>
-    <col min="7" max="7" width="56.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="47.1640625" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="37.83203125" customWidth="1"/>
+    <col min="8" max="8" width="56.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="19" thickBot="1"/>
-    <row r="2" spans="2:7" ht="19" thickBot="1">
+    <row r="1" spans="2:8" ht="19" thickBot="1"/>
+    <row r="2" spans="2:8" ht="19" thickBot="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1668,91 +1949,126 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="44">
-      <c r="B3" s="14">
+    <row r="3" spans="2:8" ht="44">
+      <c r="B3" s="20">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="15" t="s">
-        <v>13</v>
+      <c r="C3" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="70">
-      <c r="B4" s="14">
+    <row r="4" spans="2:8">
+      <c r="B4" s="12"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="2:8" ht="57">
+      <c r="B5" s="13"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="44">
+      <c r="B6" s="20">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="15" t="s">
-        <v>14</v>
+      <c r="C6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="70">
-      <c r="B5" s="14">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="15" t="s">
-        <v>15</v>
-      </c>
+    <row r="7" spans="2:8">
+      <c r="B7" s="12"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7"/>
     </row>
-    <row r="6" spans="2:7" ht="71" thickBot="1">
-      <c r="B6" s="13">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19" t="s">
-        <v>19</v>
+    <row r="8" spans="2:8" ht="71" thickBot="1">
+      <c r="B8" s="21"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="E3:E5"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Modify spec adhafera (#82)
* update system test

* update uml

* update design spec

* update version

* remove conf.py~
</commit_message>
<xml_diff>
--- a/adhafera/test/system_test.xlsx
+++ b/adhafera/test/system_test.xlsx
@@ -482,49 +482,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>・画面に"家計簿を登録しました"と書かれたToastが表示されている
-・入力欄には何も表示されていない
-・テーブルは"収入"が選択されている
-・全てのチェックマークが表示されていない</t>
-    <rPh sb="1" eb="3">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="5" eb="8">
-      <t>カケイボ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>トウロク</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="27" eb="29">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="36" eb="39">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="41" eb="42">
-      <t>ナニ</t>
-    </rPh>
-    <rPh sb="43" eb="45">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="59" eb="61">
-      <t>シュウニュウ</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="72" eb="73">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="83" eb="85">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>・入力欄には何も表示されていない
 ・テーブルは"収入"が選択されている
 ・全てのチェックマークが表示されていない</t>
@@ -574,6 +531,41 @@
       <t>スベ</t>
     </rPh>
     <rPh sb="48" eb="50">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・画面に"家計簿を登録しました"と書かれたToastが表示されている
+・日付入力欄に日付が入力されている
+・日付以外の入力欄には何も表示されていない
+・テーブルは"収入"が選択されている
+・全てのチェックマークが表示されていない</t>
+    <rPh sb="1" eb="3">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="5" eb="8">
+      <t>カケイボ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="95" eb="96">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="106" eb="108">
       <t>ヒョウジ</t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -1725,7 +1717,7 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1804,7 +1796,7 @@
         <v>24</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="57">
@@ -1849,7 +1841,7 @@
         <v>24</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="57">
@@ -1896,7 +1888,7 @@
         <v>23</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="57">
@@ -1943,7 +1935,7 @@
         <v>22</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update system test spec
</commit_message>
<xml_diff>
--- a/adhafera/test/system_test.xlsx
+++ b/adhafera/test/system_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -171,78 +171,6 @@
     </rPh>
     <rPh sb="3" eb="4">
       <t>アタイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・画面に"内容が入力されていません"と書かれたToastが表示されている
-・内容の項目にチェックマークが表示されている
-・テーブルは"収入"が選択されている</t>
-    <rPh sb="1" eb="3">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>コウモク</t>
-    </rPh>
-    <rPh sb="52" eb="54">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="67" eb="69">
-      <t>シュウニュウ</t>
-    </rPh>
-    <rPh sb="71" eb="73">
-      <t>センタク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・画面に"日付が不正です"と書かれたToastが表示されている
-・日付の項目にチェックマークが表示されている
-・テーブルは"収入"が選択されている</t>
-    <rPh sb="1" eb="3">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>フセイ</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>コウモク</t>
-    </rPh>
-    <rPh sb="47" eb="49">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="62" eb="64">
-      <t>シュウニュウ</t>
-    </rPh>
-    <rPh sb="66" eb="68">
-      <t>センタク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -382,7 +310,8 @@
     <t>・日付入力欄に日付が入力されている
 ・日付以外の入力欄には何も表示されていない
 ・テーブルは"支出"が選択されている
-・全てのチェックマークが表示されていない</t>
+・全てのチェックマークが表示されていない
+・収支が表示されている</t>
     <rPh sb="1" eb="3">
       <t>ヒヅケ</t>
     </rPh>
@@ -422,117 +351,16 @@
     <rPh sb="71" eb="73">
       <t>ヒョウジ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・日付入力欄には日付が入力されている
-・日付以外の入力欄には何も表示されていない
-・テーブルは"支出"が選択されている
-・全てのチェックマークが表示されていない</t>
-    <rPh sb="1" eb="3">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>イガイ</t>
-    </rPh>
-    <rPh sb="25" eb="28">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>ナニ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
+    <rPh sb="81" eb="83">
+      <t>シュウシ</t>
+    </rPh>
+    <rPh sb="84" eb="86">
       <t>ヒョウジ</t>
     </rPh>
-    <rPh sb="48" eb="50">
-      <t>シシュツ</t>
-    </rPh>
-    <rPh sb="52" eb="54">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="61" eb="62">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="72" eb="74">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1.1.0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1.1.0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・入力欄には何も表示されていない
-・テーブルは"収入"が選択されている
-・全てのチェックマークが表示されていない</t>
-    <rPh sb="1" eb="4">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>ナニ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>シュウニュウ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・入力欄には何も表示されていない
-・テーブルは"収入"が選択されている
-・全てのチェックマークが表示されていない</t>
-    <rPh sb="1" eb="4">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>ナニ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>シュウニュウ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>ヒョウジ</t>
-    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2.0.0</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -540,7 +368,8 @@
 ・日付入力欄に日付が入力されている
 ・日付以外の入力欄には何も表示されていない
 ・テーブルは"収入"が選択されている
-・全てのチェックマークが表示されていない</t>
+・全てのチェックマークが表示されていない
+・収支がアプリ起動時より100円増加している</t>
     <rPh sb="1" eb="3">
       <t>ガメン</t>
     </rPh>
@@ -567,6 +396,255 @@
     </rPh>
     <rPh sb="106" eb="108">
       <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="116" eb="118">
+      <t>シュウシ</t>
+    </rPh>
+    <rPh sb="122" eb="125">
+      <t>キドウジ</t>
+    </rPh>
+    <rPh sb="130" eb="131">
+      <t>エン</t>
+    </rPh>
+    <rPh sb="131" eb="133">
+      <t>ゾウカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・日付入力欄には日付が入力されている
+・日付以外の入力欄には何も表示されていない
+・テーブルは"支出"が選択されている
+・全てのチェックマークが表示されていない
+・収支が表示されている</t>
+    <rPh sb="1" eb="3">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="25" eb="28">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>シシュツ</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・入力欄には何も表示されていない
+・テーブルは"収入"が選択されている
+・全てのチェックマークが表示されていない
+・収支がアプリ起動時と同じ</t>
+    <rPh sb="1" eb="4">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="64" eb="67">
+      <t>キドウジ</t>
+    </rPh>
+    <rPh sb="68" eb="69">
+      <t>オナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・日付入力欄に日付が入力されている
+・日付以外の入力欄には何も表示されていない
+・テーブルは"支出"が選択されている
+・全てのチェックマークが表示されていない
+・収支が表示されている</t>
+    <rPh sb="1" eb="3">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="24" eb="27">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="47" eb="49">
+      <t>シシュツ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="60" eb="61">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・入力欄には何も表示されていない
+・テーブルは"収入"が選択されている
+・全てのチェックマークが表示されていない
+・収支がアプリ起動時と同じ</t>
+    <rPh sb="1" eb="4">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・画面に"内容が入力されていません"と書かれたToastが表示されている
+・内容の項目にチェックマークが表示されている
+・テーブルは"収入"が選択されている
+・収支がアプリ起動時と同じ</t>
+    <rPh sb="1" eb="3">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="67" eb="69">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・画面に"日付が不正です"と書かれたToastが表示されている
+・日付の項目にチェックマークが表示されている
+・テーブルは"収入"が選択されている
+・収支がアプリ起動時と同じ</t>
+    <rPh sb="1" eb="3">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>フセイ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="47" eb="49">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>センタク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1717,7 +1795,7 @@
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1754,12 +1832,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="57">
+    <row r="3" spans="2:8" ht="70">
       <c r="B3" s="19">
         <v>1</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>9</v>
@@ -1770,7 +1848,7 @@
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:8">
@@ -1784,7 +1862,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="2:8" ht="70">
+    <row r="5" spans="2:8" ht="83">
       <c r="B5" s="21"/>
       <c r="C5" s="13"/>
       <c r="D5" s="24"/>
@@ -1793,18 +1871,18 @@
         <v>10</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="57">
+    <row r="6" spans="2:8" ht="70">
       <c r="B6" s="25">
         <v>2</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>12</v>
@@ -1835,21 +1913,21 @@
       <c r="D8" s="24"/>
       <c r="E8" s="13"/>
       <c r="F8" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="57">
+    <row r="9" spans="2:8" ht="70">
       <c r="B9" s="25">
         <v>3</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>12</v>
@@ -1862,7 +1940,7 @@
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:8">
@@ -1876,40 +1954,40 @@
       <c r="G10" s="6"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="2:8" ht="44">
+    <row r="11" spans="2:8" ht="57">
       <c r="B11" s="21"/>
       <c r="C11" s="13"/>
       <c r="D11" s="24"/>
       <c r="E11" s="18"/>
       <c r="F11" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="57">
+    <row r="12" spans="2:8" ht="70">
       <c r="B12" s="25">
         <v>4</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:8">
@@ -1932,10 +2010,10 @@
         <v>7</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2010,12 +2088,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="57">
+    <row r="3" spans="2:8" ht="70">
       <c r="B3" s="25">
         <v>1</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>9</v>
@@ -2028,7 +2106,7 @@
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:8">
@@ -2042,7 +2120,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="2:8" ht="57">
+    <row r="5" spans="2:8" ht="70">
       <c r="B5" s="21"/>
       <c r="C5" s="13"/>
       <c r="D5" s="24"/>
@@ -2051,18 +2129,18 @@
         <v>10</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="57">
+    <row r="6" spans="2:8" ht="70">
       <c r="B6" s="25">
         <v>2</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>9</v>
@@ -2075,7 +2153,7 @@
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:8">
@@ -2098,10 +2176,10 @@
         <v>10</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>